<commit_message>
#2 update report basic info
</commit_message>
<xml_diff>
--- a/Safeway/wwwroot/exportTemplate/小微评审内容.xlsx
+++ b/Safeway/wwwroot/exportTemplate/小微评审内容.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bettyzhao\Desktop\exportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bettyzhao\Documents\GitHub\Safeway\Safeway\wwwroot\exportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1574,71 +1574,71 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1958,8 +1958,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="71" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="71" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,16 +1977,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:12" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1998,28 +1998,28 @@
         <v>190</v>
       </c>
       <c r="D2" s="28"/>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="25"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="44"/>
       <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:12" s="24" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="28"/>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="25"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
       <c r="I3" s="44"/>
       <c r="J3" s="48"/>
     </row>
@@ -2064,13 +2064,13 @@
       <c r="J5" s="48"/>
     </row>
     <row r="6" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="62" t="s">
         <v>176</v>
       </c>
       <c r="D6" s="29" t="s">
@@ -2093,9 +2093,9 @@
       <c r="L6" s="48"/>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="51"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="55"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="32" t="s">
         <v>174</v>
       </c>
@@ -2115,11 +2115,11 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="51"/>
-      <c r="B8" s="49" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="60" t="s">
         <v>171</v>
       </c>
       <c r="D8" s="35" t="s">
@@ -2141,9 +2141,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="51"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="51"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="35" t="s">
         <v>168</v>
       </c>
@@ -2163,8 +2163,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" s="5" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="51"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="33" t="s">
         <v>166</v>
       </c>
@@ -2187,8 +2187,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="51"/>
-      <c r="B11" s="49" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="53" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="33" t="s">
@@ -2213,8 +2213,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="51"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="33" t="s">
         <v>159</v>
       </c>
@@ -2237,8 +2237,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57" t="s">
+      <c r="A13" s="66"/>
+      <c r="B13" s="66" t="s">
         <v>156</v>
       </c>
       <c r="C13" s="33" t="s">
@@ -2263,8 +2263,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1" ht="229.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="9" t="s">
         <v>152</v>
       </c>
@@ -2287,8 +2287,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
         <v>149</v>
       </c>
@@ -2311,8 +2311,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="33" t="s">
         <v>146</v>
       </c>
@@ -2335,11 +2335,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="58"/>
-      <c r="B17" s="50" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="60" t="s">
         <v>142</v>
       </c>
       <c r="D17" s="35" t="s">
@@ -2361,9 +2361,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="58"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="56"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="32" t="s">
         <v>139</v>
       </c>
@@ -2383,8 +2383,8 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="58"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="33" t="s">
         <v>137</v>
       </c>
@@ -2407,8 +2407,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" s="5" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="57"/>
-      <c r="B20" s="57"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="9" t="s">
         <v>134</v>
       </c>
@@ -2431,8 +2431,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" s="5" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="33" t="s">
         <v>131</v>
       </c>
@@ -2455,8 +2455,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="58"/>
-      <c r="B22" s="49" t="s">
+      <c r="A22" s="67"/>
+      <c r="B22" s="53" t="s">
         <v>128</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -2481,8 +2481,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A23" s="58"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="9" t="s">
         <v>124</v>
       </c>
@@ -2505,8 +2505,8 @@
       </c>
     </row>
     <row r="24" spans="1:10" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="58"/>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="67"/>
+      <c r="B24" s="60" t="s">
         <v>121</v>
       </c>
       <c r="C24" s="29" t="s">
@@ -2531,8 +2531,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" s="5" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="59"/>
-      <c r="B25" s="56"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="64"/>
       <c r="C25" s="9" t="s">
         <v>117</v>
       </c>
@@ -2555,9 +2555,9 @@
       </c>
     </row>
     <row r="26" spans="1:10" s="5" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="50" t="s">
+      <c r="A26" s="66"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="60" t="s">
         <v>114</v>
       </c>
       <c r="D26" s="35" t="s">
@@ -2579,9 +2579,9 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="5" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="58"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="51"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="35" t="s">
         <v>194</v>
       </c>
@@ -2601,10 +2601,10 @@
       </c>
     </row>
     <row r="28" spans="1:10" s="5" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="60" t="s">
         <v>109</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -2629,9 +2629,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" s="5" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="58"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="50" t="s">
+      <c r="A29" s="67"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="60" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="32" t="s">
@@ -2653,9 +2653,9 @@
       </c>
     </row>
     <row r="30" spans="1:10" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.15">
-      <c r="A30" s="58"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="32" t="s">
         <v>102</v>
       </c>
@@ -2675,9 +2675,9 @@
       </c>
     </row>
     <row r="31" spans="1:10" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.15">
-      <c r="A31" s="59"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="32" t="s">
         <v>100</v>
       </c>
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.15">
-      <c r="A32" s="57"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="34" t="s">
@@ -2719,11 +2719,11 @@
       </c>
     </row>
     <row r="33" spans="1:10" s="5" customFormat="1" ht="156.94999999999999" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="58"/>
-      <c r="B33" s="50" t="s">
+      <c r="A33" s="67"/>
+      <c r="B33" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="66" t="s">
         <v>95</v>
       </c>
       <c r="D33" s="32" t="s">
@@ -2745,9 +2745,9 @@
       </c>
     </row>
     <row r="34" spans="1:10" s="5" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="58"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="58"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="67"/>
       <c r="D34" s="32" t="s">
         <v>93</v>
       </c>
@@ -2767,9 +2767,9 @@
       </c>
     </row>
     <row r="35" spans="1:10" s="5" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="58"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="58"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="67"/>
       <c r="D35" s="32" t="s">
         <v>92</v>
       </c>
@@ -2789,9 +2789,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" s="5" customFormat="1" ht="89.25" x14ac:dyDescent="0.15">
-      <c r="A36" s="59"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="59"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="68"/>
       <c r="D36" s="32" t="s">
         <v>91</v>
       </c>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="37" spans="1:10" s="5" customFormat="1" ht="150.94999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="19"/>
-      <c r="B37" s="57"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="17"/>
       <c r="D37" s="32" t="s">
         <v>90</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="38" spans="1:10" s="5" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="19"/>
-      <c r="B38" s="59"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="15"/>
       <c r="D38" s="32" t="s">
         <v>89</v>
@@ -2855,9 +2855,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" s="5" customFormat="1" ht="260.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="57"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
       <c r="D39" s="32" t="s">
         <v>88</v>
       </c>
@@ -2877,9 +2877,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" s="5" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="59"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
       <c r="D40" s="34" t="s">
         <v>87</v>
       </c>
@@ -2899,8 +2899,8 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="5" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="57"/>
-      <c r="B41" s="57"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="66"/>
       <c r="C41" s="17"/>
       <c r="D41" s="32" t="s">
         <v>86</v>
@@ -2921,8 +2921,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="58"/>
-      <c r="B42" s="58"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="16"/>
       <c r="D42" s="32" t="s">
         <v>84</v>
@@ -2943,8 +2943,8 @@
       </c>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="58"/>
-      <c r="B43" s="58"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="16"/>
       <c r="D43" s="32" t="s">
         <v>83</v>
@@ -2965,8 +2965,8 @@
       </c>
     </row>
     <row r="44" spans="1:10" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="58"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="16"/>
       <c r="D44" s="32" t="s">
         <v>82</v>
@@ -2987,8 +2987,8 @@
       </c>
     </row>
     <row r="45" spans="1:10" s="5" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="59"/>
-      <c r="B45" s="59"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="68"/>
       <c r="C45" s="15"/>
       <c r="D45" s="32" t="s">
         <v>81</v>
@@ -3009,9 +3009,9 @@
       </c>
     </row>
     <row r="46" spans="1:10" s="5" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="50" t="s">
+      <c r="A46" s="66"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="60" t="s">
         <v>80</v>
       </c>
       <c r="D46" s="35" t="s">
@@ -3033,9 +3033,9 @@
       </c>
     </row>
     <row r="47" spans="1:10" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="59"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="56"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="32" t="s">
         <v>77</v>
       </c>
@@ -3055,8 +3055,8 @@
       </c>
     </row>
     <row r="48" spans="1:10" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="57"/>
-      <c r="B48" s="57"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="9" t="s">
         <v>75</v>
       </c>
@@ -3079,8 +3079,8 @@
       </c>
     </row>
     <row r="49" spans="1:10" s="5" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="58"/>
-      <c r="B49" s="58"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="36" t="s">
         <v>73</v>
       </c>
@@ -3103,13 +3103,13 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="5" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="50" t="s">
+      <c r="A50" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="60" t="s">
         <v>68</v>
       </c>
       <c r="D50" s="32" t="s">
@@ -3131,9 +3131,9 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="5" customFormat="1" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="51"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="56"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="32" t="s">
         <v>66</v>
       </c>
@@ -3153,9 +3153,9 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="5" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="51"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="54" t="s">
+      <c r="A52" s="61"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="62" t="s">
         <v>65</v>
       </c>
       <c r="D52" s="35" t="s">
@@ -3177,9 +3177,9 @@
       </c>
     </row>
     <row r="53" spans="1:10" s="5" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="51"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="55"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="65"/>
       <c r="D53" s="32" t="s">
         <v>62</v>
       </c>
@@ -3199,8 +3199,8 @@
       </c>
     </row>
     <row r="54" spans="1:10" s="5" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="51"/>
-      <c r="B54" s="49" t="s">
+      <c r="A54" s="61"/>
+      <c r="B54" s="53" t="s">
         <v>60</v>
       </c>
       <c r="C54" s="33" t="s">
@@ -3225,9 +3225,9 @@
       </c>
     </row>
     <row r="55" spans="1:10" s="5" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="51"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="54" t="s">
+      <c r="A55" s="61"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="62" t="s">
         <v>56</v>
       </c>
       <c r="D55" s="35" t="s">
@@ -3249,9 +3249,9 @@
       </c>
     </row>
     <row r="56" spans="1:10" s="5" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="51"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="60"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="38" t="s">
         <v>53</v>
       </c>
@@ -3271,8 +3271,8 @@
       </c>
     </row>
     <row r="57" spans="1:10" s="5" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="50"/>
-      <c r="B57" s="49" t="s">
+      <c r="A57" s="60"/>
+      <c r="B57" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -3297,8 +3297,8 @@
       </c>
     </row>
     <row r="58" spans="1:10" s="5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="51"/>
-      <c r="B58" s="49"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="53"/>
       <c r="C58" s="9" t="s">
         <v>48</v>
       </c>
@@ -3321,11 +3321,11 @@
       </c>
     </row>
     <row r="59" spans="1:10" s="5" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="51"/>
-      <c r="B59" s="49" t="s">
+      <c r="A59" s="61"/>
+      <c r="B59" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="49" t="s">
+      <c r="C59" s="53" t="s">
         <v>45</v>
       </c>
       <c r="D59" s="35" t="s">
@@ -3347,9 +3347,9 @@
       </c>
     </row>
     <row r="60" spans="1:10" s="5" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="51"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="49"/>
+      <c r="A60" s="61"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
       <c r="D60" s="35" t="s">
         <v>42</v>
       </c>
@@ -3369,13 +3369,13 @@
       </c>
     </row>
     <row r="61" spans="1:10" s="5" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="61" t="s">
+      <c r="A61" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="64" t="s">
+      <c r="B61" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="58" t="s">
         <v>38</v>
       </c>
       <c r="D61" s="38" t="s">
@@ -3397,9 +3397,9 @@
       </c>
     </row>
     <row r="62" spans="1:10" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="62"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="66"/>
+      <c r="A62" s="55"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="59"/>
       <c r="D62" s="32" t="s">
         <v>35</v>
       </c>
@@ -3419,8 +3419,8 @@
       </c>
     </row>
     <row r="63" spans="1:10" s="5" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="63"/>
-      <c r="B63" s="64"/>
+      <c r="A63" s="56"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="13" t="s">
         <v>33</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.15">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="53" t="s">
         <v>26</v>
       </c>
       <c r="B65" s="32" t="s">
@@ -3497,11 +3497,11 @@
       </c>
     </row>
     <row r="66" spans="1:10" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.15">
-      <c r="A66" s="49"/>
-      <c r="B66" s="49" t="s">
+      <c r="A66" s="53"/>
+      <c r="B66" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="53" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="32" t="s">
@@ -3523,9 +3523,9 @@
       </c>
     </row>
     <row r="67" spans="1:10" s="5" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="49"/>
-      <c r="B67" s="49"/>
-      <c r="C67" s="49"/>
+      <c r="A67" s="53"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="53"/>
       <c r="D67" s="35" t="s">
         <v>18</v>
       </c>
@@ -3545,11 +3545,11 @@
       </c>
     </row>
     <row r="68" spans="1:10" s="5" customFormat="1" ht="45.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="49"/>
-      <c r="B68" s="49" t="s">
+      <c r="A68" s="53"/>
+      <c r="B68" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" s="53" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -3571,9 +3571,9 @@
       </c>
     </row>
     <row r="69" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="49"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="49"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
       <c r="D69" s="35" t="s">
         <v>12</v>
       </c>
@@ -3593,10 +3593,10 @@
       </c>
     </row>
     <row r="70" spans="1:10" s="5" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="49" t="s">
+      <c r="B70" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="9" t="s">
@@ -3621,8 +3621,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="49"/>
-      <c r="B71" s="49"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="53"/>
       <c r="C71" s="9" t="s">
         <v>6</v>
       </c>
@@ -3645,7 +3645,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" s="5" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="49"/>
+      <c r="A72" s="53"/>
       <c r="B72" s="32" t="s">
         <v>4</v>
       </c>
@@ -3671,20 +3671,20 @@
       </c>
     </row>
     <row r="73" spans="1:10" s="5" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="67" t="s">
+      <c r="A73" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="68"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="69"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="51"/>
       <c r="E73" s="6">
         <f>SUM(E6:E72)</f>
         <v>600</v>
       </c>
-      <c r="F73" s="67" t="s">
+      <c r="F73" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G73" s="70"/>
+      <c r="G73" s="52"/>
       <c r="H73" s="42"/>
       <c r="I73" s="46"/>
       <c r="J73" s="48"/>
@@ -3692,6 +3692,59 @@
   </sheetData>
   <autoFilter ref="I1:I85"/>
   <mergeCells count="62">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
     <mergeCell ref="A73:D73"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="A70:A72"/>
@@ -3701,59 +3754,6 @@
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3785,7 +3785,7 @@
 </file>
 
 <file path=customXml/item10.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5iTSI5UodjD94nh7U7VklxY>fbkDatHo10yHfCS/coEENSGgVnA0jHuR5p3SijxupcQx8tAlarjoczNNPvmIsLMFzG15pBlYe08WcFTMGuwWVA==</nXeGKudETKPeaCNGFh5iTSI5UodjD94nh7U7VklxY>
+<nXeGKudETKPeaCNGFh5iTSI5UodjD94nh7U7VklxY>0W2GXKy1VbSiyNz+OnYcdhN2a4JUoM6nd4zXsPFp7QDkzGkVrTG5g20ahaubJ3tZEknMHRtlkFfUV0wSM+q0QQ==</nXeGKudETKPeaCNGFh5iTSI5UodjD94nh7U7VklxY>
 </file>
 
 <file path=customXml/item11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3813,11 +3813,11 @@
 </file>
 
 <file path=customXml/item17.xml><?xml version="1.0" encoding="utf-8"?>
-<NovaPath_docIDOld>686B6ATJ4HWMIJ4ULT2YVBBH8B</NovaPath_docIDOld>
+<NovaPath_docIDOld>9JZRDT1GOCUQWFGWKY3RDASKJF</NovaPath_docIDOld>
 </file>
 
 <file path=customXml/item18.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5i5JKJLOqxkMZWB6LsYfMaI9RtbpE1WkCpXazESWus5B>XrTT552/pKC+eWLaOycDgxu3uEosOCCWSbdeZNvTBvE1TXb3rv2hrDrvyXT0nAvCaaVAnQNw5EaMy8XGKgI1Pg==</nXeGKudETKPeaCNGFh5i5JKJLOqxkMZWB6LsYfMaI9RtbpE1WkCpXazESWus5B>
+<nXeGKudETKPeaCNGFh5i5JKJLOqxkMZWB6LsYfMaI9RtbpE1WkCpXazESWus5B>fbkDatHo10yHfCS/coEENSGgVnA0jHuR5p3SijxupcQx8tAlarjoczNNPvmIsLMFzG15pBlYe08WcFTMGuwWVA==</nXeGKudETKPeaCNGFh5i5JKJLOqxkMZWB6LsYfMaI9RtbpE1WkCpXazESWus5B>
 </file>
 
 <file path=customXml/item19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3825,7 +3825,7 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5iy53cs4YTjZQd4Re9Stbph13fJwq3N1dxRUwfkxNCzGbktJIbKf2q8mQyY814Q>GoBUcRQBOiWNv9cnqy33XA==</nXeGKudETKPeaCNGFh5iy53cs4YTjZQd4Re9Stbph13fJwq3N1dxRUwfkxNCzGbktJIbKf2q8mQyY814Q>
+<nXeGKudETKPeaCNGFh5i2aVdoOsLYjULCdH7T707tDyRRmguot4fEcJ2iD6f9>aijtZbeaDr5ifuku6q8Dl4KnAmxHbEzlw2o+upnhWGM=</nXeGKudETKPeaCNGFh5i2aVdoOsLYjULCdH7T707tDyRRmguot4fEcJ2iD6f9>
 </file>
 
 <file path=customXml/item20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3861,27 +3861,27 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5i2aVdoOsLYjULCdH7T707tDyRRmguot4fEcJ2iD6f9>aijtZbeaDr5ifuku6q8Dl4KnAmxHbEzlw2o+upnhWGM=</nXeGKudETKPeaCNGFh5i2aVdoOsLYjULCdH7T707tDyRRmguot4fEcJ2iD6f9>
+<nXeGKudETKPeaCNGFh5iy53cs4YTjZQd4Re9Stbph13fJwq3N1dxRUwfkxNCzGbktJIbKf2q8mQyY814Q>GoBUcRQBOiWNv9cnqy33XA==</nXeGKudETKPeaCNGFh5iy53cs4YTjZQd4Re9Stbph13fJwq3N1dxRUwfkxNCzGbktJIbKf2q8mQyY814Q>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<NovaPath_docPath>C:\Users\bettyzhao\Desktop\exportTemplate</NovaPath_docPath>
+<NovaPath_docPath>C:\Users\bettyzhao\Documents\GitHub\Safeway\Safeway\wwwroot\exportTemplate</NovaPath_docPath>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5i0BGlH9ci87cLWvMx3DlPzuAPh2gY9s703zKUS7uW>mZ4rtFSXbzk2Ux9ca9oo0+MEa0nHGRvM3YnrG9+VxUkROD/lpW0KT18j9ONtFnkJxFeLpNM9p/iCm8B604o0hnM/vHNa44GJ5YbYEx+B+Uyz9vkRl0wymbLv2/pBfrjC</nXeGKudETKPeaCNGFh5i0BGlH9ci87cLWvMx3DlPzuAPh2gY9s703zKUS7uW>
+<nXeGKudETKPeaCNGFh5i0BGlH9ci87cLWvMx3DlPzuAPh2gY9s703zKUS7uW>mZ4rtFSXbzk2Ux9ca9oo0+MEa0nHGRvM3YnrG9+VxUmBDDpZAyEOJMSoXK/26JdzVMp5WPaNthSrg5FCkzXxvXqw+ctjtp1x5pja/9Bc/+Is51SAHKzNddxnt1ovNgdtmPnk0XXhc+d0YtT+N9vLsl09OGRuhwXzVTkr3s4whJD+/PKqLA7nhHA+jA3JxZ8zLiS2rS3rItUgOX8pEtLRsQ==</nXeGKudETKPeaCNGFh5i0BGlH9ci87cLWvMx3DlPzuAPh2gY9s703zKUS7uW>
 </file>
 
 <file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
-<NovaPath_docName>C:\Users\bettyzhao\Desktop\exportTemplate\小微评审.xlsx</NovaPath_docName>
+<NovaPath_docName>C:\Users\bettyzhao\Documents\GitHub\Safeway\Safeway\wwwroot\exportTemplate\小微评审内容.xlsx</NovaPath_docName>
 </file>
 
 <file path=customXml/item8.xml><?xml version="1.0" encoding="utf-8"?>
-<nXeGKudETKPeaCNGFh5i7cKyawAjgyQn9gyiebCxx1jD9eHXSWW9Lib2F1j9>mZ4rtFSXbzk2Ux9ca9oo0+MEa0nHGRvM3YnrG9+VxUkROD/lpW0KT18j9ONtFnkJxFeLpNM9p/iCm8B604o0hnM/vHNa44GJ5YbYEx+B+UzYRFe4/mfBEVf7yAAoORXHw8CyEwGdQCCAXI21rZmhHw==</nXeGKudETKPeaCNGFh5i7cKyawAjgyQn9gyiebCxx1jD9eHXSWW9Lib2F1j9>
+<nXeGKudETKPeaCNGFh5i7cKyawAjgyQn9gyiebCxx1jD9eHXSWW9Lib2F1j9>mZ4rtFSXbzk2Ux9ca9oo0+MEa0nHGRvM3YnrG9+VxUmBDDpZAyEOJMSoXK/26JdzVMp5WPaNthSrg5FCkzXxvXqw+ctjtp1x5pja/9Bc/+Is51SAHKzNddxnt1ovNgdtmPnk0XXhc+d0YtT+N9vLsl09OGRuhwXzVTkr3s4whJD+/PKqLA7nhHA+jA3JxZ8zkQbkpEvnVMKnC2gXkNxIaTn3cT0qHrQrWsUkbQH9Etc=</nXeGKudETKPeaCNGFh5i7cKyawAjgyQn9gyiebCxx1jD9eHXSWW9Lib2F1j9>
 </file>
 
 <file path=customXml/item9.xml><?xml version="1.0" encoding="utf-8"?>
-<NovaPath_docID>9JZRDT1GOCUQWFGWKY3RDASKJF</NovaPath_docID>
+<NovaPath_docID>84ZP0OP0ILE8AJHEDMG1KUQW3X</NovaPath_docID>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3891,109 +3891,109 @@
 </file>
 
 <file path=customXml/itemProps10.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50B327D8-B6E7-4043-B199-A3AAD79B2526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{873ABBCB-2F7F-4208-8F22-19366308D088}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps11.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{202B5724-8AC4-43D0-82B7-ABCBDAAF9077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C6287CE-2482-48F2-A262-74814E18D923}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps12.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33FFD718-5788-478F-A118-DE550777D53F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D3C52B-5E76-4867-AC41-E0BA1272347C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps13.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D5A4648-E784-4126-872A-80A2CA790922}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44DCEAB-16B9-4302-896B-BC40B6E5EDF5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps14.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3A7BD3F-6FA2-489D-B30F-AF090CEDF8DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DBC6C5C-12F8-459D-9E54-7931D0423A33}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps15.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0CE0FA-F883-4FEF-B42E-DDBF7E4CDCAC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C79B81A-D9B1-481F-8B58-D89FCDFCEE87}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps16.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CC0694-CF78-4D5F-8DA8-F817506FC5BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B22987E-2201-4252-8686-9AC1294E0277}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps17.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C621C5-FDB9-4AF1-B7BA-80013832988F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B2133B4-4D7F-4463-BA1C-C927342AA594}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps18.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E3B4978-595A-45A0-911B-0E1C19C14F29}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C29C9A2-C41A-43F8-806D-1ABD02813400}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps19.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E2674C9-4889-436D-A389-4B43ACB0FCBD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044822AF-2BB8-4357-9426-FDE5068BA96B}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA82C119-EE81-4E19-BFC8-648830FF3AE0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01CF30C1-4959-4D3A-B180-0B8F5A0AA3A1}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps20.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF30987-A304-4E03-A22A-CE3D4B5C0246}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6EA3B7-9765-4482-B864-0C240349FB7F}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps21.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD5D7574-66C7-4FB8-8587-BA647D814333}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC9673D0-7D4D-4363-A49B-8073A45D5FC3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps22.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58BD71AD-34A5-42D7-9925-23F4DC5DBCD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1E4D475-D94C-4E84-83F0-3039E38262C3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps23.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF32D50E-35CA-47A2-B1D2-3FFF67F91034}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2A094E-0A1A-4758-A45D-DFC5B9FA592A}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps24.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15C5AC18-4714-4214-B016-C303944085D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C33C314-3432-416C-98AD-CA33080D5079}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps25.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00EE7DB1-FF05-49AB-BAB1-6846A0A3B2ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A4F1B8-0B36-4140-B0AA-3D23DE5ABBA8}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps26.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72EFBFEB-F0C1-40B9-A5C7-F44193A70FE3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{303FDF75-7378-4C6A-8BAE-C1ABCEEB2B4D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -4005,37 +4005,37 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01CF30C1-4959-4D3A-B180-0B8F5A0AA3A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA82C119-EE81-4E19-BFC8-648830FF3AE0}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE70B7ED-AD3C-4A09-BAA3-17DD11AE0E5A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1605FD99-9A82-43D9-85D5-306E0B748225}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B99202BB-5A06-416E-AE68-938C8C20212A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{057324FA-6092-4B0A-AE3C-2CFADC4C02F1}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFBD72FE-E553-40EC-B245-2C7DA01808CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70713A35-6B09-4629-847C-B04553A4FDEA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps8.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA2BF3D-3C85-445B-9B55-441094551827}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6FEA9A1-81EE-410E-A57A-1068EF9F6E39}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps9.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{556EBCB9-33F1-4201-BCF9-975094A8D02F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83B7CE3-7F55-4658-A46C-18A56EC32EE7}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>